<commit_message>
Revised rubric and isntructions
</commit_message>
<xml_diff>
--- a/Labs/Lab02/CS133JS_Lab02_Rubrics.xlsx
+++ b/Labs/Lab02/CS133JS_Lab02_Rubrics.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\CS133JS-CourseMaterials\Labs\Lab02\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D5C566A-EDD5-4C74-85C4-D07F314C0957}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0D3E119-8A0E-4F58-A8B9-8E09E4F37B11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32760" yWindow="4896" windowWidth="15744" windowHeight="11208" activeTab="2" xr2:uid="{9702CE45-50CE-F14F-802C-E5FE921247A2}"/>
+    <workbookView xWindow="11388" yWindow="1860" windowWidth="17556" windowHeight="13008" activeTab="1" xr2:uid="{9702CE45-50CE-F14F-802C-E5FE921247A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Group A" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="27">
   <si>
     <t>Criteria</t>
   </si>
@@ -103,6 +103,21 @@
   </si>
   <si>
     <t>Function exercises in the console</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    I/O is done in the web page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Code quality</t>
+  </si>
+  <si>
+    <t>Uses parseFloat, GetElementById</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Uses parseFloat, GetElementById</t>
+  </si>
+  <si>
+    <t>Function exercises</t>
   </si>
 </sst>
 </file>
@@ -154,12 +169,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -474,10 +488,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3216228F-B421-8943-9C69-C9FAC1E7C520}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7:E14"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -485,15 +499,15 @@
     <col min="3" max="3" width="17.69921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -504,129 +518,246 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="4">
+        <v>26</v>
+      </c>
+      <c r="D5">
         <v>10</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="4">
-        <v>2</v>
-      </c>
-      <c r="E7" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8">
         <v>5</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="J8">
+        <v>5</v>
+      </c>
+      <c r="K8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9">
+        <v>4</v>
+      </c>
+      <c r="E9">
+        <v>4</v>
+      </c>
+      <c r="J9">
+        <v>4</v>
+      </c>
+      <c r="K9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="E10">
+        <v>2</v>
+      </c>
+      <c r="J10">
+        <v>2</v>
+      </c>
+      <c r="K10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+      <c r="E11">
+        <v>2</v>
+      </c>
+      <c r="J11">
+        <v>4</v>
+      </c>
+      <c r="K11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+      <c r="E12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13">
         <v>8</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E13">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="4">
-        <v>4</v>
-      </c>
-      <c r="E10" s="4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" s="4">
-        <v>10</v>
-      </c>
-      <c r="E11" s="4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="J13">
+        <v>2</v>
+      </c>
+      <c r="K13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="4">
-        <v>6</v>
-      </c>
-      <c r="E12" s="4">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="D14">
+        <v>4</v>
+      </c>
+      <c r="E14">
+        <v>4</v>
+      </c>
+      <c r="J14">
+        <v>8</v>
+      </c>
+      <c r="K14">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
+      <c r="E15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+      <c r="E16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D17">
+        <v>2</v>
+      </c>
+      <c r="E17">
+        <v>2</v>
+      </c>
+      <c r="J17">
+        <v>4</v>
+      </c>
+      <c r="K17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="4">
+      <c r="D18">
         <v>3</v>
       </c>
-      <c r="E13" s="4">
+      <c r="E18">
         <v>3</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="J18">
+        <v>3</v>
+      </c>
+      <c r="K18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>18</v>
       </c>
-      <c r="D14" s="4">
-        <v>2</v>
-      </c>
-      <c r="E14" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+      <c r="D19">
+        <v>2</v>
+      </c>
+      <c r="E19">
+        <v>2</v>
+      </c>
+      <c r="J19">
+        <v>2</v>
+      </c>
+      <c r="K19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J20">
+        <v>2</v>
+      </c>
+      <c r="K20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>3</v>
       </c>
-      <c r="D16">
-        <f>SUM(D5:D14)</f>
+      <c r="D21">
+        <f>SUM(D5:D19)</f>
         <v>50</v>
       </c>
-      <c r="E16">
-        <f>SUM(E5:E14)</f>
+      <c r="E21">
+        <f>SUM(E5:E19)</f>
         <v>50</v>
       </c>
     </row>
@@ -638,26 +769,28 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45DD923E-8052-6149-B2F0-947B5BE982A5}">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5:E5"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="17.69921875" customWidth="1"/>
+    <col min="3" max="3" width="20.8984375" customWidth="1"/>
+    <col min="4" max="4" width="7.59765625" customWidth="1"/>
+    <col min="5" max="5" width="6.296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -668,32 +801,32 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5">
         <v>10</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -704,7 +837,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -715,86 +848,132 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9">
+        <v>4</v>
+      </c>
+      <c r="E9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="E10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11">
+        <v>4</v>
+      </c>
+      <c r="E11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+      <c r="E12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13">
         <v>8</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E13">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="4">
-        <v>4</v>
-      </c>
-      <c r="E10" s="4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11">
-        <v>10</v>
-      </c>
-      <c r="E11">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>9</v>
       </c>
-      <c r="D12">
-        <v>6</v>
-      </c>
-      <c r="E12">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="D14">
+        <v>4</v>
+      </c>
+      <c r="E14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>11</v>
       </c>
-      <c r="D13">
+      <c r="D15">
         <v>3</v>
       </c>
-      <c r="E13">
+      <c r="E15">
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+      <c r="E16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D17">
+        <v>2</v>
+      </c>
+      <c r="E17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>18</v>
       </c>
-      <c r="D14">
-        <v>2</v>
-      </c>
-      <c r="E14">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+      <c r="D19">
+        <v>2</v>
+      </c>
+      <c r="E19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F20" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>3</v>
       </c>
-      <c r="D16">
-        <f>SUM(D5:D14)</f>
+      <c r="D21">
+        <f>SUM(D5:D19)</f>
         <v>50</v>
       </c>
-      <c r="E16">
-        <f>SUM(E5:E14)</f>
+      <c r="E21">
+        <f>SUM(E5:E19)</f>
         <v>50</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -804,10 +983,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44F5606A-302D-8F40-B769-19B85F064B34}">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -845,10 +1024,10 @@
       <c r="A5" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5">
         <v>10</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5">
         <v>10</v>
       </c>
     </row>
@@ -856,17 +1035,15 @@
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="4">
-        <v>2</v>
-      </c>
-      <c r="E7" s="4">
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7">
         <v>2</v>
       </c>
     </row>
@@ -874,10 +1051,10 @@
       <c r="A8" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8">
         <v>5</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8">
         <v>5</v>
       </c>
     </row>
@@ -885,82 +1062,126 @@
       <c r="A9" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="4">
-        <v>8</v>
-      </c>
-      <c r="E9" s="4">
-        <v>8</v>
+      <c r="D9">
+        <v>4</v>
+      </c>
+      <c r="E9">
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="4">
-        <v>4</v>
-      </c>
-      <c r="E10" s="4">
-        <v>4</v>
+        <v>22</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="E10">
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="D11">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="E11">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="D12">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E12">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="D13">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E13">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="D14">
         <v>2</v>
       </c>
       <c r="E14">
         <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15">
+        <v>4</v>
+      </c>
+      <c r="E15">
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16">
         <v>3</v>
       </c>
-      <c r="D16">
-        <f>SUM(D5:D14)</f>
-        <v>50</v>
-      </c>
       <c r="E16">
-        <f>SUM(E5:E14)</f>
-        <v>50</v>
+        <v>3</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D17">
+        <v>2</v>
+      </c>
+      <c r="E17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18">
+        <v>2</v>
+      </c>
+      <c r="E18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>3</v>
+      </c>
+      <c r="D20">
+        <f>SUM(D5:D18)</f>
+        <v>50</v>
+      </c>
+      <c r="E20">
+        <f>SUM(E5:E18)</f>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating rubric... in process
</commit_message>
<xml_diff>
--- a/Labs/Lab02/CS133JS_Lab02_Rubrics.xlsx
+++ b/Labs/Lab02/CS133JS_Lab02_Rubrics.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\CS133JS-CourseMaterials\Labs\Lab02\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/birdb/Projects/CS133JS-CourseMaterials/Labs/Lab02/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0D3E119-8A0E-4F58-A8B9-8E09E4F37B11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0605C9C-A785-E24F-92AC-0158D6FF1E98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11388" yWindow="1860" windowWidth="17556" windowHeight="13008" activeTab="1" xr2:uid="{9702CE45-50CE-F14F-802C-E5FE921247A2}"/>
+    <workbookView xWindow="-20380" yWindow="2820" windowWidth="20340" windowHeight="15340" xr2:uid="{9702CE45-50CE-F14F-802C-E5FE921247A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Group A" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="31">
   <si>
     <t>Criteria</t>
   </si>
@@ -118,6 +118,18 @@
   </si>
   <si>
     <t>Function exercises</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>name, date comments in each file</t>
+  </si>
+  <si>
+    <t>Excelent work!</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Here's the grade breakedown:</t>
   </si>
 </sst>
 </file>
@@ -169,11 +181,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -488,280 +509,263 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3216228F-B421-8943-9C69-C9FAC1E7C520}">
-  <dimension ref="A1:K21"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="17.69921875" customWidth="1"/>
+    <col min="1" max="1" width="31.5" customWidth="1"/>
+    <col min="2" max="2" width="7.33203125" customWidth="1"/>
+    <col min="3" max="3" width="5.33203125" customWidth="1"/>
+    <col min="4" max="4" width="1.5" customWidth="1"/>
+    <col min="5" max="5" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="1"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="B4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="C4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>26</v>
       </c>
-      <c r="D5">
+      <c r="B6">
         <v>10</v>
       </c>
-      <c r="E5">
+      <c r="C6">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+      <c r="E6" s="4"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="E7" s="4"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="E8" s="4"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="E9" s="4"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>3</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
+      <c r="E10" s="4"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="E11" s="4"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="E12" s="4"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="E13" s="4"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14">
         <v>6</v>
       </c>
-      <c r="D7">
-        <v>2</v>
-      </c>
-      <c r="E7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8">
-        <v>5</v>
-      </c>
-      <c r="E8">
-        <v>5</v>
-      </c>
-      <c r="J8">
-        <v>5</v>
-      </c>
-      <c r="K8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="C14">
+        <v>6</v>
+      </c>
+      <c r="E14" s="4"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>9</v>
       </c>
-      <c r="D9">
-        <v>4</v>
-      </c>
-      <c r="E9">
-        <v>4</v>
-      </c>
-      <c r="J9">
-        <v>4</v>
-      </c>
-      <c r="K9">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="B15">
+        <v>3</v>
+      </c>
+      <c r="C15">
+        <v>3</v>
+      </c>
+      <c r="E15" s="4"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="E16" s="4"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>22</v>
       </c>
-      <c r="D10">
-        <v>2</v>
-      </c>
-      <c r="E10">
-        <v>2</v>
-      </c>
-      <c r="J10">
-        <v>2</v>
-      </c>
-      <c r="K10">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11">
-        <v>2</v>
-      </c>
-      <c r="E11">
-        <v>2</v>
-      </c>
-      <c r="J11">
-        <v>4</v>
-      </c>
-      <c r="K11">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+      <c r="E17" s="4"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>23</v>
       </c>
-      <c r="D12">
-        <v>2</v>
-      </c>
-      <c r="E12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13">
-        <v>8</v>
-      </c>
-      <c r="E13">
-        <v>8</v>
-      </c>
-      <c r="J13">
-        <v>2</v>
-      </c>
-      <c r="K13">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>9</v>
-      </c>
-      <c r="D14">
-        <v>4</v>
-      </c>
-      <c r="E14">
-        <v>4</v>
-      </c>
-      <c r="J14">
-        <v>8</v>
-      </c>
-      <c r="K14">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>24</v>
-      </c>
-      <c r="D15">
-        <v>2</v>
-      </c>
-      <c r="E15">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>22</v>
-      </c>
-      <c r="D16">
-        <v>2</v>
-      </c>
-      <c r="E16">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>23</v>
-      </c>
-      <c r="D17">
-        <v>2</v>
-      </c>
-      <c r="E17">
-        <v>2</v>
-      </c>
-      <c r="J17">
-        <v>4</v>
-      </c>
-      <c r="K17">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="E18" s="4"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>11</v>
       </c>
-      <c r="D18">
-        <v>3</v>
-      </c>
-      <c r="E18">
-        <v>3</v>
-      </c>
-      <c r="J18">
-        <v>3</v>
-      </c>
-      <c r="K18">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="E19" s="4"/>
+    </row>
+    <row r="20" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D19">
-        <v>2</v>
-      </c>
-      <c r="E19">
-        <v>2</v>
-      </c>
-      <c r="J19">
-        <v>2</v>
-      </c>
-      <c r="K19">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="J20">
-        <v>2</v>
-      </c>
-      <c r="K20">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>3</v>
-      </c>
-      <c r="D21">
-        <f>SUM(D5:D19)</f>
-        <v>50</v>
-      </c>
-      <c r="E21">
-        <f>SUM(E5:E19)</f>
-        <v>50</v>
-      </c>
+      <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
+      <c r="E20" s="4"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E21" s="4"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>3</v>
+      </c>
+      <c r="B22">
+        <f>SUM(B6:B20)</f>
+        <v>40</v>
+      </c>
+      <c r="C22">
+        <f>SUM(C6:C20)</f>
+        <v>40</v>
+      </c>
+      <c r="E22" s="4"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A3:E3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -771,26 +775,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45DD923E-8052-6149-B2F0-947B5BE982A5}">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView topLeftCell="B4" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="20.8984375" customWidth="1"/>
-    <col min="4" max="4" width="7.59765625" customWidth="1"/>
-    <col min="5" max="5" width="6.296875" customWidth="1"/>
+    <col min="3" max="3" width="20.83203125" customWidth="1"/>
+    <col min="4" max="4" width="7.6640625" customWidth="1"/>
+    <col min="5" max="5" width="6.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -801,16 +805,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="D5">
         <v>10</v>
@@ -819,14 +823,14 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -837,7 +841,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -848,7 +852,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -859,7 +863,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -870,7 +874,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>25</v>
       </c>
@@ -881,7 +885,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -892,7 +896,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -903,7 +907,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -914,7 +918,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -925,7 +929,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -936,7 +940,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -947,7 +951,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -955,15 +959,15 @@
         <v>2</v>
       </c>
       <c r="E19">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F20" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>3</v>
       </c>
@@ -973,7 +977,7 @@
       </c>
       <c r="E21">
         <f>SUM(E5:E19)</f>
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -985,24 +989,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44F5606A-302D-8F40-B769-19B85F064B34}">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView topLeftCell="A5" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="17.69921875" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -1013,14 +1017,14 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -1031,12 +1035,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1047,7 +1051,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -1058,7 +1062,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1069,7 +1073,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -1080,7 +1084,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1091,7 +1095,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -1102,7 +1106,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -1113,7 +1117,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>22</v>
       </c>
@@ -1124,7 +1128,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>9</v>
       </c>
@@ -1135,7 +1139,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>11</v>
       </c>
@@ -1149,7 +1153,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -1160,7 +1164,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -1171,7 +1175,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
Updated the rubric for fall 23
</commit_message>
<xml_diff>
--- a/Labs/Lab02/CS133JS_Lab02_Rubrics.xlsx
+++ b/Labs/Lab02/CS133JS_Lab02_Rubrics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/birdb/Projects/CS133JS-CourseMaterials/Labs/Lab02/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0605C9C-A785-E24F-92AC-0158D6FF1E98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B775B18-E4D7-5D42-9109-31A94577EF55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-20380" yWindow="2820" windowWidth="20340" windowHeight="15340" xr2:uid="{9702CE45-50CE-F14F-802C-E5FE921247A2}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="33">
   <si>
     <t>Criteria</t>
   </si>
@@ -57,9 +57,6 @@
     <t>Part 2</t>
   </si>
   <si>
-    <t>Developer’s name, date in comments in each file</t>
-  </si>
-  <si>
     <t>Multiple choice quiz</t>
   </si>
   <si>
@@ -130,6 +127,15 @@
   </si>
   <si>
     <t xml:space="preserve"> Here's the grade breakedown:</t>
+  </si>
+  <si>
+    <t>Name, date in comments in each file</t>
+  </si>
+  <si>
+    <t>Excellent work!</t>
+  </si>
+  <si>
+    <t>Here's the grade breakdown:</t>
   </si>
 </sst>
 </file>
@@ -181,7 +187,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -189,12 +195,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -512,7 +523,7 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -526,26 +537,26 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
@@ -558,7 +569,7 @@
         <v>2</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -570,7 +581,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B6">
         <v>10</v>
@@ -590,7 +601,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -602,7 +613,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
         <v>3</v>
@@ -614,7 +625,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
         <v>3</v>
@@ -626,7 +637,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B11">
         <v>2</v>
@@ -638,7 +649,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B12">
         <v>2</v>
@@ -650,7 +661,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -662,7 +673,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B14">
         <v>6</v>
@@ -674,7 +685,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B15">
         <v>3</v>
@@ -686,7 +697,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B16">
         <v>2</v>
@@ -698,7 +709,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B17">
         <v>2</v>
@@ -710,7 +721,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -722,7 +733,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B19">
         <v>2</v>
@@ -734,7 +745,7 @@
     </row>
     <row r="20" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B20">
         <v>2</v>
@@ -773,422 +784,526 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45DD923E-8052-6149-B2F0-947B5BE982A5}">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView topLeftCell="B4" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="20.83203125" customWidth="1"/>
-    <col min="4" max="4" width="7.6640625" customWidth="1"/>
-    <col min="5" max="5" width="6.33203125" customWidth="1"/>
+    <col min="1" max="1" width="31.33203125" customWidth="1"/>
+    <col min="2" max="2" width="7.83203125" customWidth="1"/>
+    <col min="3" max="3" width="6.1640625" customWidth="1"/>
+    <col min="4" max="4" width="1.1640625" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="1"/>
+      <c r="A2" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="A3" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5">
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6">
         <v>10</v>
       </c>
-      <c r="E5">
+      <c r="C6">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+      <c r="E6" s="4"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7">
-        <v>2</v>
-      </c>
-      <c r="E7">
-        <v>2</v>
-      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="E7" s="4"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8">
-        <v>5</v>
-      </c>
-      <c r="E8">
-        <v>5</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="E8" s="4"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9">
-        <v>4</v>
-      </c>
-      <c r="E9">
-        <v>4</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="E9" s="4"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10">
-        <v>2</v>
-      </c>
-      <c r="E10">
-        <v>2</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>3</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
+      <c r="E10" s="4"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11">
-        <v>4</v>
-      </c>
-      <c r="E11">
-        <v>4</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="E11" s="4"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12">
-        <v>2</v>
-      </c>
-      <c r="E12">
-        <v>2</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="E12" s="4"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>19</v>
-      </c>
-      <c r="D13">
-        <v>8</v>
-      </c>
-      <c r="E13">
-        <v>8</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="E13" s="4"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>9</v>
-      </c>
-      <c r="D14">
-        <v>4</v>
-      </c>
-      <c r="E14">
-        <v>4</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="B14">
+        <v>6</v>
+      </c>
+      <c r="C14">
+        <v>6</v>
+      </c>
+      <c r="E14" s="4"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>11</v>
-      </c>
-      <c r="D15">
-        <v>3</v>
-      </c>
-      <c r="E15">
-        <v>3</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="B15">
+        <v>3</v>
+      </c>
+      <c r="C15">
+        <v>3</v>
+      </c>
+      <c r="E15" s="4"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>22</v>
-      </c>
-      <c r="D16">
-        <v>2</v>
-      </c>
-      <c r="E16">
-        <v>2</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="E16" s="4"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>23</v>
-      </c>
-      <c r="D17">
-        <v>2</v>
-      </c>
-      <c r="E17">
-        <v>2</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+      <c r="E17" s="4"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="E18" s="4"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>18</v>
-      </c>
-      <c r="D19">
-        <v>2</v>
-      </c>
-      <c r="E19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="F20" s="3" t="s">
-        <v>13</v>
-      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="E19" s="4"/>
+    </row>
+    <row r="20" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A20" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
+      <c r="E20" s="4"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>3</v>
-      </c>
-      <c r="D21">
-        <f>SUM(D5:D19)</f>
-        <v>50</v>
-      </c>
-      <c r="E21">
-        <f>SUM(E5:E19)</f>
-        <v>48</v>
-      </c>
+      <c r="E21" s="4"/>
+      <c r="F21" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>3</v>
+      </c>
+      <c r="B22">
+        <f>SUM(B6:B20)</f>
+        <v>40</v>
+      </c>
+      <c r="C22">
+        <f>SUM(C6:C20)</f>
+        <v>40</v>
+      </c>
+      <c r="E22" s="4"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A3:E3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44F5606A-302D-8F40-B769-19B85F064B34}">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="17.6640625" customWidth="1"/>
+    <col min="1" max="1" width="39" customWidth="1"/>
+    <col min="2" max="2" width="7.83203125" customWidth="1"/>
+    <col min="3" max="3" width="5.83203125" customWidth="1"/>
+    <col min="4" max="4" width="1" customWidth="1"/>
+    <col min="5" max="5" width="20.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6">
+        <v>10</v>
+      </c>
+      <c r="C6">
+        <v>10</v>
+      </c>
+      <c r="E6" s="4"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="E7" s="4"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="E8" s="4"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="1"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="E9" s="4"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>3</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
+      <c r="E10" s="4"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>21</v>
       </c>
-      <c r="D5">
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="E11" s="4"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="E12" s="4"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="E13" s="4"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14">
+        <v>6</v>
+      </c>
+      <c r="C14">
+        <v>6</v>
+      </c>
+      <c r="E14" s="4"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15">
+        <v>3</v>
+      </c>
+      <c r="C15">
+        <v>3</v>
+      </c>
+      <c r="E15" s="4"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="E16" s="4"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>10</v>
       </c>
-      <c r="E5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7">
-        <v>2</v>
-      </c>
-      <c r="E7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8">
-        <v>5</v>
-      </c>
-      <c r="E8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9">
-        <v>4</v>
-      </c>
-      <c r="E9">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+      <c r="E17" s="4"/>
+      <c r="F17" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>22</v>
       </c>
-      <c r="D10">
-        <v>2</v>
-      </c>
-      <c r="E10">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11">
-        <v>4</v>
-      </c>
-      <c r="E11">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12">
-        <v>2</v>
-      </c>
-      <c r="E12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="E18" s="4"/>
+    </row>
+    <row r="19" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D13">
-        <v>8</v>
-      </c>
-      <c r="E13">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>22</v>
-      </c>
-      <c r="D14">
-        <v>2</v>
-      </c>
-      <c r="E14">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>9</v>
-      </c>
-      <c r="D15">
-        <v>4</v>
-      </c>
-      <c r="E15">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>11</v>
-      </c>
-      <c r="D16">
-        <v>3</v>
-      </c>
-      <c r="E16">
-        <v>3</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>23</v>
-      </c>
-      <c r="D17">
-        <v>2</v>
-      </c>
-      <c r="E17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>18</v>
-      </c>
-      <c r="D18">
-        <v>2</v>
-      </c>
-      <c r="E18">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>3</v>
-      </c>
-      <c r="D20">
-        <f>SUM(D5:D18)</f>
-        <v>50</v>
-      </c>
-      <c r="E20">
-        <f>SUM(E5:E18)</f>
-        <v>50</v>
-      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="E19" s="4"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
+      <c r="E20" s="4"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21" s="4"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B22">
+        <f>SUM(B6:B20)</f>
+        <v>40</v>
+      </c>
+      <c r="C22">
+        <f>SUM(C6:C20)</f>
+        <v>40</v>
+      </c>
+      <c r="E22" s="4"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A3:E3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Tweaks to the rubric
</commit_message>
<xml_diff>
--- a/Labs/Lab02/CS133JS_Lab02_Rubrics.xlsx
+++ b/Labs/Lab02/CS133JS_Lab02_Rubrics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/birdb/Projects/CS133JS-CourseMaterials/Labs/Lab02/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B775B18-E4D7-5D42-9109-31A94577EF55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A1319E4-5960-FF43-8219-7CD7180F9F40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20380" yWindow="2820" windowWidth="20340" windowHeight="15340" xr2:uid="{9702CE45-50CE-F14F-802C-E5FE921247A2}"/>
+    <workbookView xWindow="-21700" yWindow="4620" windowWidth="21200" windowHeight="16800" activeTab="1" xr2:uid="{9702CE45-50CE-F14F-802C-E5FE921247A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Group A" sheetId="1" r:id="rId1"/>
@@ -126,9 +126,6 @@
     <t>Excelent work!</t>
   </si>
   <si>
-    <t xml:space="preserve"> Here's the grade breakedown:</t>
-  </si>
-  <si>
     <t>Name, date in comments in each file</t>
   </si>
   <si>
@@ -136,6 +133,9 @@
   </si>
   <si>
     <t>Here's the grade breakdown:</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Here's the grade breakdown:</t>
   </si>
 </sst>
 </file>
@@ -195,17 +195,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -522,8 +526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3216228F-B421-8943-9C69-C9FAC1E7C520}">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -540,23 +544,23 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:5" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+    </row>
+    <row r="3" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
@@ -786,8 +790,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45DD923E-8052-6149-B2F0-947B5BE982A5}">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -804,23 +808,23 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="9" t="s">
+    <row r="2" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+    </row>
+    <row r="3" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
@@ -865,7 +869,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -1005,7 +1009,7 @@
       <c r="E19" s="4"/>
     </row>
     <row r="20" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A20" s="8" t="s">
+      <c r="A20" s="5" t="s">
         <v>17</v>
       </c>
       <c r="B20">
@@ -1050,7 +1054,7 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="A3" sqref="A3:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1067,23 +1071,23 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:5" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+    </row>
+    <row r="3" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
@@ -1128,7 +1132,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B8">
         <v>1</v>

</xml_diff>

<commit_message>
Minor format changes to the rubric spreadsheet
</commit_message>
<xml_diff>
--- a/Labs/Lab02/CS133JS_Lab02_Rubrics.xlsx
+++ b/Labs/Lab02/CS133JS_Lab02_Rubrics.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/birdb/Projects/CS133JS-CourseMaterials/Labs/Lab02/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\CS133JS-CourseMaterials\Labs\Lab02\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8729E59E-0355-4A4A-9D8A-0F15583B6C97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10B00F9C-DC97-4CF7-A16B-DE5D5DB5C431}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21700" yWindow="4620" windowWidth="21200" windowHeight="16800" xr2:uid="{9702CE45-50CE-F14F-802C-E5FE921247A2}"/>
+    <workbookView xWindow="-11676" yWindow="4212" windowWidth="11664" windowHeight="12216" activeTab="2" xr2:uid="{9702CE45-50CE-F14F-802C-E5FE921247A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Group A" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="35">
   <si>
     <t>Criteria</t>
   </si>
@@ -99,9 +99,6 @@
     <t>Cost per mile app functionality</t>
   </si>
   <si>
-    <t>Function exercises in the console</t>
-  </si>
-  <si>
     <t xml:space="preserve">    I/O is done in the web page</t>
   </si>
   <si>
@@ -129,9 +126,6 @@
     <t>Name, date in comments in each file</t>
   </si>
   <si>
-    <t>Excellent work!</t>
-  </si>
-  <si>
     <t>Here's the grade breakdown:</t>
   </si>
   <si>
@@ -142,6 +136,12 @@
   </si>
   <si>
     <t xml:space="preserve">Excellent work! </t>
+  </si>
+  <si>
+    <t>Part 2: Excellent work!</t>
+  </si>
+  <si>
+    <t>Part 1: Excellent job of completing the exercises!</t>
   </si>
 </sst>
 </file>
@@ -193,7 +193,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -211,17 +211,19 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -240,9 +242,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -280,7 +282,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -386,7 +388,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -528,7 +530,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -538,43 +540,47 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3216228F-B421-8943-9C69-C9FAC1E7C520}">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView topLeftCell="A15" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="31.5" customWidth="1"/>
-    <col min="2" max="2" width="7.33203125" customWidth="1"/>
-    <col min="3" max="3" width="5.33203125" customWidth="1"/>
+    <col min="2" max="2" width="7.296875" customWidth="1"/>
+    <col min="3" max="3" width="5.296875" customWidth="1"/>
     <col min="4" max="4" width="1.5" customWidth="1"/>
     <col min="5" max="5" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="12" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+    </row>
+    <row r="2" spans="1:5" ht="49.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
     </row>
-    <row r="3" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -585,19 +591,19 @@
         <v>2</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B6">
         <v>10</v>
@@ -607,7 +613,7 @@
       </c>
       <c r="E6" s="4"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -615,9 +621,9 @@
       <c r="C7" s="2"/>
       <c r="E7" s="4"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -627,7 +633,7 @@
       </c>
       <c r="E8" s="4"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -639,7 +645,7 @@
       </c>
       <c r="E9" s="4"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -651,34 +657,34 @@
       </c>
       <c r="E10" s="4"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="E11" s="4"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="E12" s="4"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>21</v>
       </c>
-      <c r="B11">
-        <v>2</v>
-      </c>
-      <c r="C11">
-        <v>2</v>
-      </c>
-      <c r="E11" s="4"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>23</v>
-      </c>
-      <c r="B12">
-        <v>2</v>
-      </c>
-      <c r="C12">
-        <v>2</v>
-      </c>
-      <c r="E12" s="4"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>22</v>
-      </c>
       <c r="B13">
         <v>1</v>
       </c>
@@ -687,7 +693,7 @@
       </c>
       <c r="E13" s="4"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>6</v>
       </c>
@@ -699,7 +705,7 @@
       </c>
       <c r="E14" s="4"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -711,9 +717,9 @@
       </c>
       <c r="E15" s="4"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B16">
         <v>2</v>
@@ -723,22 +729,22 @@
       </c>
       <c r="E16" s="4"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+      <c r="E17" s="4"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>21</v>
       </c>
-      <c r="B17">
-        <v>2</v>
-      </c>
-      <c r="C17">
-        <v>2</v>
-      </c>
-      <c r="E17" s="4"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>22</v>
-      </c>
       <c r="B18">
         <v>1</v>
       </c>
@@ -747,7 +753,7 @@
       </c>
       <c r="E18" s="4"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>10</v>
       </c>
@@ -759,7 +765,7 @@
       </c>
       <c r="E19" s="4"/>
     </row>
-    <row r="20" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>17</v>
       </c>
@@ -771,10 +777,10 @@
       </c>
       <c r="E20" s="4"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E21" s="4"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>3</v>
       </c>
@@ -789,9 +795,10 @@
       <c r="E22" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A1:E1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -806,39 +813,39 @@
       <selection activeCell="A2" sqref="A2:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31.33203125" customWidth="1"/>
-    <col min="2" max="2" width="7.83203125" customWidth="1"/>
-    <col min="3" max="3" width="6.1640625" customWidth="1"/>
-    <col min="4" max="4" width="1.1640625" customWidth="1"/>
-    <col min="5" max="5" width="15.33203125" customWidth="1"/>
+    <col min="1" max="1" width="31.296875" customWidth="1"/>
+    <col min="2" max="2" width="7.796875" customWidth="1"/>
+    <col min="3" max="3" width="6.19921875" customWidth="1"/>
+    <col min="4" max="4" width="1.19921875" customWidth="1"/>
+    <col min="5" max="5" width="15.296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-    </row>
-    <row r="3" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+    </row>
+    <row r="3" spans="1:5" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -849,19 +856,19 @@
         <v>2</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B6">
         <v>10</v>
@@ -871,7 +878,7 @@
       </c>
       <c r="E6" s="4"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -879,9 +886,9 @@
       <c r="C7" s="2"/>
       <c r="E7" s="4"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -891,7 +898,7 @@
       </c>
       <c r="E8" s="4"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -903,7 +910,7 @@
       </c>
       <c r="E9" s="4"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -915,34 +922,34 @@
       </c>
       <c r="E10" s="4"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="E11" s="4"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="E12" s="4"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>21</v>
       </c>
-      <c r="B11">
-        <v>2</v>
-      </c>
-      <c r="C11">
-        <v>2</v>
-      </c>
-      <c r="E11" s="4"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>24</v>
-      </c>
-      <c r="B12">
-        <v>2</v>
-      </c>
-      <c r="C12">
-        <v>2</v>
-      </c>
-      <c r="E12" s="4"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>22</v>
-      </c>
       <c r="B13">
         <v>1</v>
       </c>
@@ -951,7 +958,7 @@
       </c>
       <c r="E13" s="4"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -963,7 +970,7 @@
       </c>
       <c r="E14" s="4"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -975,7 +982,7 @@
       </c>
       <c r="E15" s="4"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>10</v>
       </c>
@@ -987,9 +994,9 @@
       </c>
       <c r="E16" s="4"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B17">
         <v>2</v>
@@ -999,9 +1006,9 @@
       </c>
       <c r="E17" s="4"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -1011,9 +1018,9 @@
       </c>
       <c r="E18" s="4"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B19">
         <v>2</v>
@@ -1023,7 +1030,7 @@
       </c>
       <c r="E19" s="4"/>
     </row>
-    <row r="20" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>17</v>
       </c>
@@ -1035,13 +1042,13 @@
       </c>
       <c r="E20" s="4"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E21" s="4"/>
       <c r="F21" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>3</v>
       </c>
@@ -1066,265 +1073,280 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44F5606A-302D-8F40-B769-19B85F064B34}">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="39" customWidth="1"/>
-    <col min="2" max="2" width="7.83203125" customWidth="1"/>
-    <col min="3" max="3" width="5.83203125" customWidth="1"/>
+    <col min="2" max="2" width="7.796875" customWidth="1"/>
+    <col min="3" max="3" width="5.796875" customWidth="1"/>
     <col min="4" max="4" width="1" customWidth="1"/>
-    <col min="5" max="5" width="20.1640625" customWidth="1"/>
+    <col min="5" max="5" width="20.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="12" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-    </row>
-    <row r="3" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="8" t="s">
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+    </row>
+    <row r="2" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+    </row>
+    <row r="3" spans="1:5" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+    </row>
+    <row r="4" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7">
+        <v>10</v>
+      </c>
+      <c r="C7">
+        <v>10</v>
+      </c>
+      <c r="E7" s="4"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="E8" s="4"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="E9" s="4"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10">
+        <v>3</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
+      <c r="E10" s="4"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="C11">
+        <v>3</v>
+      </c>
+      <c r="E11" s="4"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="E12" s="4"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="E13" s="4"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="E14" s="4"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15">
+        <v>6</v>
+      </c>
+      <c r="C15">
+        <v>6</v>
+      </c>
+      <c r="E15" s="4"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
+      </c>
+      <c r="C16">
+        <v>3</v>
+      </c>
+      <c r="E16" s="4"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+      <c r="E17" s="4"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6">
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="C18">
+        <v>2</v>
+      </c>
+      <c r="E18" s="4"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>10</v>
       </c>
-      <c r="C6">
-        <v>10</v>
-      </c>
-      <c r="E6" s="4"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="E7" s="4"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="E8" s="4"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9">
-        <v>3</v>
-      </c>
-      <c r="C9">
-        <v>3</v>
-      </c>
-      <c r="E9" s="4"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10">
-        <v>3</v>
-      </c>
-      <c r="C10">
-        <v>3</v>
-      </c>
-      <c r="E10" s="4"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="E19" s="4"/>
+      <c r="F19" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>21</v>
       </c>
-      <c r="B11">
-        <v>2</v>
-      </c>
-      <c r="C11">
-        <v>2</v>
-      </c>
-      <c r="E11" s="4"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12">
-        <v>2</v>
-      </c>
-      <c r="C12">
-        <v>2</v>
-      </c>
-      <c r="E12" s="4"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13">
-        <v>1</v>
-      </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
-      <c r="E13" s="4"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14">
-        <v>6</v>
-      </c>
-      <c r="C14">
-        <v>6</v>
-      </c>
-      <c r="E14" s="4"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>21</v>
-      </c>
-      <c r="B15">
-        <v>3</v>
-      </c>
-      <c r="C15">
-        <v>3</v>
-      </c>
-      <c r="E15" s="4"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>8</v>
-      </c>
-      <c r="B16">
-        <v>2</v>
-      </c>
-      <c r="C16">
-        <v>2</v>
-      </c>
-      <c r="E16" s="4"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>33</v>
-      </c>
-      <c r="B17">
-        <v>2</v>
-      </c>
-      <c r="C17">
-        <v>2</v>
-      </c>
-      <c r="E17" s="4"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>10</v>
-      </c>
-      <c r="B18">
-        <v>2</v>
-      </c>
-      <c r="C18">
-        <v>2</v>
-      </c>
-      <c r="E18" s="4"/>
-      <c r="F18" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>22</v>
-      </c>
-      <c r="B19">
-        <v>1</v>
-      </c>
-      <c r="C19">
-        <v>1</v>
-      </c>
-      <c r="E19" s="4"/>
-    </row>
-    <row r="20" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A20" s="4" t="s">
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="E20" s="4"/>
+    </row>
+    <row r="21" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A21" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B20">
-        <v>2</v>
-      </c>
-      <c r="C20">
-        <v>2</v>
-      </c>
-      <c r="E20" s="4"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>3</v>
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
       </c>
       <c r="E21" s="4"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B22">
-        <f>SUM(B6:B20)</f>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E22" s="4"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23">
+        <f>SUM(B7:B21)</f>
         <v>40</v>
       </c>
-      <c r="C22">
-        <f>SUM(C6:C20)</f>
+      <c r="C23">
+        <f>SUM(C7:C21)</f>
         <v>40</v>
       </c>
-      <c r="E22" s="4"/>
+      <c r="E23" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
+    <mergeCell ref="A3:E3"/>
     <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="A1:E1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>